<commit_message>
Versiones 3, 4 y 5
CoNA
</commit_message>
<xml_diff>
--- a/Proyecto Interno/Time-series/mapeo_retail_sipsa.xlsx
+++ b/Proyecto Interno/Time-series/mapeo_retail_sipsa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8f89820ab55adc2/Escritorio/Least-cost-diets-and-affordability/Proyecto Interno/Time-series/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{8B350617-12E7-48A3-8EB9-7DC4E59CA7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71F011E1-856F-419F-BD47-AE474E7966C1}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8B350617-12E7-48A3-8EB9-7DC4E59CA7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C8FF6AF-1091-42EF-9978-523BFE9BC29D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F9B8AFAB-AE7C-4ECE-8124-D73A073E0F9D}"/>
   </bookViews>
@@ -1465,10 +1465,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0188B28-EF9D-41DB-9815-3D89235996E0}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:B276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F146" sqref="F146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1485,7 +1486,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1515,7 +1516,7 @@
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1547,7 +1548,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1555,7 +1556,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1601,7 +1602,7 @@
       </c>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1616,7 @@
       </c>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
@@ -1735,7 +1736,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>22</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
@@ -1791,7 +1792,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>23</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>23</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>24</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>25</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>25</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>25</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>25</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>25</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>25</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>25</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>25</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>25</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>25</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>25</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>25</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>25</v>
       </c>
@@ -1975,7 +1976,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>26</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>27</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>27</v>
       </c>
@@ -1999,7 +2000,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>27</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>27</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>27</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>27</v>
       </c>
@@ -2031,7 +2032,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>27</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>27</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>28</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>28</v>
       </c>
@@ -2071,7 +2072,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>28</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>28</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>28</v>
       </c>
@@ -2095,7 +2096,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>29</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
@@ -2125,7 +2126,7 @@
       </c>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>33</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>34</v>
       </c>
@@ -2141,7 +2142,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>35</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>35</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>35</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>35</v>
       </c>
@@ -2173,7 +2174,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>35</v>
       </c>
@@ -2181,7 +2182,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>35</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>35</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>35</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>35</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>35</v>
       </c>
@@ -2221,7 +2222,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>35</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>35</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>35</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>35</v>
       </c>
@@ -2259,7 +2260,7 @@
       </c>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>37</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>38</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>39</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>39</v>
       </c>
@@ -2291,7 +2292,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>39</v>
       </c>
@@ -2299,7 +2300,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>39</v>
       </c>
@@ -2307,7 +2308,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>39</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>39</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>40</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>41</v>
       </c>
@@ -2339,7 +2340,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>41</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>42</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>43</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>44</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>44</v>
       </c>
@@ -2379,7 +2380,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>44</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>44</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>44</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>44</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>44</v>
       </c>
@@ -2419,7 +2420,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>44</v>
       </c>
@@ -2427,7 +2428,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>45</v>
       </c>
@@ -2459,7 +2460,7 @@
       </c>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>50</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>50</v>
       </c>
@@ -2475,7 +2476,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>51</v>
       </c>
@@ -2483,7 +2484,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>51</v>
       </c>
@@ -2491,7 +2492,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>52</v>
       </c>
@@ -2499,7 +2500,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>52</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>52</v>
       </c>
@@ -2515,7 +2516,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>52</v>
       </c>
@@ -2523,7 +2524,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>52</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>53</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>54</v>
       </c>
@@ -2547,7 +2548,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>54</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>55</v>
       </c>
@@ -2563,7 +2564,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>55</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>55</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>55</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>55</v>
       </c>
@@ -2595,7 +2596,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>55</v>
       </c>
@@ -2603,7 +2604,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>55</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>55</v>
       </c>
@@ -2631,7 +2632,7 @@
       </c>
       <c r="B147" s="2"/>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>58</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>58</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>58</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>58</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>59</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>59</v>
       </c>
@@ -2679,7 +2680,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>59</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>59</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>59</v>
       </c>
@@ -2715,7 +2716,7 @@
       </c>
       <c r="B158" s="2"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>62</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>63</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>63</v>
       </c>
@@ -2739,7 +2740,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>63</v>
       </c>
@@ -2747,7 +2748,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>64</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>64</v>
       </c>
@@ -2763,7 +2764,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>64</v>
       </c>
@@ -2789,7 +2790,7 @@
       </c>
       <c r="B168" s="2"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>68</v>
       </c>
@@ -2797,7 +2798,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>68</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>68</v>
       </c>
@@ -2813,7 +2814,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>68</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>68</v>
       </c>
@@ -2829,7 +2830,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>69</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>69</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>69</v>
       </c>
@@ -2853,7 +2854,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>69</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>69</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>69</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>69</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>69</v>
       </c>
@@ -2893,7 +2894,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>69</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>69</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>69</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>69</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>69</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>69</v>
       </c>
@@ -2941,7 +2942,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>69</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>69</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>69</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>70</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>70</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>70</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>71</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>71</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>71</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>71</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>71</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>71</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>72</v>
       </c>
@@ -3051,7 +3052,7 @@
       </c>
       <c r="B201" s="2"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>74</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>74</v>
       </c>
@@ -3067,7 +3068,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>74</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>74</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>74</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>74</v>
       </c>
@@ -3099,7 +3100,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>74</v>
       </c>
@@ -3107,7 +3108,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>74</v>
       </c>
@@ -3115,7 +3116,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>74</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>75</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>75</v>
       </c>
@@ -3139,7 +3140,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>75</v>
       </c>
@@ -3147,7 +3148,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>75</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>75</v>
       </c>
@@ -3163,7 +3164,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>75</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>75</v>
       </c>
@@ -3179,7 +3180,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>75</v>
       </c>
@@ -3187,7 +3188,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>75</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>75</v>
       </c>
@@ -3203,7 +3204,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>75</v>
       </c>
@@ -3211,7 +3212,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>75</v>
       </c>
@@ -3219,7 +3220,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>75</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>75</v>
       </c>
@@ -3241,7 +3242,7 @@
       </c>
       <c r="B225" s="2"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>77</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>77</v>
       </c>
@@ -3257,7 +3258,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>78</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>78</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>78</v>
       </c>
@@ -3281,7 +3282,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>78</v>
       </c>
@@ -3289,7 +3290,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>78</v>
       </c>
@@ -3297,7 +3298,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>78</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>78</v>
       </c>
@@ -3313,7 +3314,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>78</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>78</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>78</v>
       </c>
@@ -3337,7 +3338,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>79</v>
       </c>
@@ -3345,7 +3346,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>79</v>
       </c>
@@ -3353,7 +3354,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>79</v>
       </c>
@@ -3361,7 +3362,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>79</v>
       </c>
@@ -3369,7 +3370,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>79</v>
       </c>
@@ -3377,7 +3378,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>79</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>79</v>
       </c>
@@ -3393,7 +3394,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>80</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>80</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>80</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>80</v>
       </c>
@@ -3425,7 +3426,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>81</v>
       </c>
@@ -3433,7 +3434,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>82</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>82</v>
       </c>
@@ -3449,7 +3450,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>82</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>82</v>
       </c>
@@ -3465,7 +3466,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>82</v>
       </c>
@@ -3473,7 +3474,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>83</v>
       </c>
@@ -3481,7 +3482,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>84</v>
       </c>
@@ -3489,7 +3490,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>84</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>85</v>
       </c>
@@ -3505,7 +3506,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>85</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>85</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>85</v>
       </c>
@@ -3529,7 +3530,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>85</v>
       </c>
@@ -3537,7 +3538,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>85</v>
       </c>
@@ -3545,7 +3546,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>85</v>
       </c>
@@ -3553,7 +3554,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>85</v>
       </c>
@@ -3561,7 +3562,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>85</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>86</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>87</v>
       </c>
@@ -3591,7 +3592,7 @@
       </c>
       <c r="B269" s="2"/>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>89</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>89</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>89</v>
       </c>
@@ -3615,7 +3616,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>89</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>90</v>
       </c>
@@ -3631,7 +3632,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>90</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>90</v>
       </c>
@@ -3648,7 +3649,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B276" xr:uid="{A49E52AF-D615-4580-8F94-DDCBB3E7D289}"/>
+  <autoFilter ref="A1:B276" xr:uid="{A49E52AF-D615-4580-8F94-DDCBB3E7D289}">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>